<commit_message>
Modified 05/08/2024 04:58:10 PM IST
</commit_message>
<xml_diff>
--- a/Extracted Data/VRU Headform (C) - Color-wise data/2022_cars_combined.xlsx
+++ b/Extracted Data/VRU Headform (C) - Color-wise data/2022_cars_combined.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J67"/>
+  <dimension ref="A1:J66"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1656,29 +1656,29 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t xml:space="preserve">VW Polo 2022 </t>
+          <t xml:space="preserve">Nissan Ariya 2022 </t>
         </is>
       </c>
       <c r="B36" t="n">
-        <v>10.13</v>
+        <v>0</v>
       </c>
       <c r="C36" t="n">
-        <v>21.52</v>
+        <v>29.41</v>
       </c>
       <c r="D36" t="n">
-        <v>33.54</v>
+        <v>36.47</v>
       </c>
       <c r="E36" t="n">
-        <v>15.19</v>
+        <v>11.76</v>
       </c>
       <c r="F36" t="n">
-        <v>8.23</v>
+        <v>8.82</v>
       </c>
       <c r="G36" t="n">
-        <v>5.06</v>
+        <v>10</v>
       </c>
       <c r="H36" t="n">
-        <v>6.33</v>
+        <v>3.53</v>
       </c>
       <c r="I36" t="n">
         <v>0</v>
@@ -1690,29 +1690,29 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t xml:space="preserve">Nissan Ariya 2022 </t>
+          <t xml:space="preserve">smart 1 2022 </t>
         </is>
       </c>
       <c r="B37" t="n">
-        <v>0</v>
+        <v>1.79</v>
       </c>
       <c r="C37" t="n">
-        <v>29.41</v>
+        <v>22.62</v>
       </c>
       <c r="D37" t="n">
-        <v>36.47</v>
+        <v>34.52</v>
       </c>
       <c r="E37" t="n">
-        <v>11.76</v>
+        <v>19.05</v>
       </c>
       <c r="F37" t="n">
-        <v>8.82</v>
+        <v>8.93</v>
       </c>
       <c r="G37" t="n">
-        <v>10</v>
+        <v>10.71</v>
       </c>
       <c r="H37" t="n">
-        <v>3.53</v>
+        <v>2.38</v>
       </c>
       <c r="I37" t="n">
         <v>0</v>
@@ -1724,29 +1724,29 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t xml:space="preserve">smart 1 2022 </t>
+          <t xml:space="preserve">Hyundai IONIQ 6 2022 </t>
         </is>
       </c>
       <c r="B38" t="n">
-        <v>1.79</v>
+        <v>4.49</v>
       </c>
       <c r="C38" t="n">
-        <v>22.62</v>
+        <v>3.37</v>
       </c>
       <c r="D38" t="n">
-        <v>34.52</v>
+        <v>14.04</v>
       </c>
       <c r="E38" t="n">
-        <v>19.05</v>
+        <v>36.52</v>
       </c>
       <c r="F38" t="n">
-        <v>8.93</v>
+        <v>20.22</v>
       </c>
       <c r="G38" t="n">
-        <v>10.71</v>
+        <v>17.98</v>
       </c>
       <c r="H38" t="n">
-        <v>2.38</v>
+        <v>3.37</v>
       </c>
       <c r="I38" t="n">
         <v>0</v>
@@ -1758,29 +1758,29 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t xml:space="preserve">Hyundai IONIQ 6 2022 </t>
+          <t xml:space="preserve">Toyota Corolla Cross 2022 </t>
         </is>
       </c>
       <c r="B39" t="n">
-        <v>4.49</v>
+        <v>0</v>
       </c>
       <c r="C39" t="n">
-        <v>3.37</v>
+        <v>45.83</v>
       </c>
       <c r="D39" t="n">
-        <v>14.04</v>
+        <v>34.52</v>
       </c>
       <c r="E39" t="n">
-        <v>36.52</v>
+        <v>11.31</v>
       </c>
       <c r="F39" t="n">
-        <v>20.22</v>
+        <v>2.38</v>
       </c>
       <c r="G39" t="n">
-        <v>17.98</v>
+        <v>3.57</v>
       </c>
       <c r="H39" t="n">
-        <v>3.37</v>
+        <v>2.38</v>
       </c>
       <c r="I39" t="n">
         <v>0</v>
@@ -1792,29 +1792,29 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t xml:space="preserve">Toyota Corolla Cross 2022 </t>
+          <t xml:space="preserve">Range Rover Sport 2022 </t>
         </is>
       </c>
       <c r="B40" t="n">
         <v>0</v>
       </c>
       <c r="C40" t="n">
-        <v>45.83</v>
+        <v>31.67</v>
       </c>
       <c r="D40" t="n">
-        <v>34.52</v>
+        <v>23.89</v>
       </c>
       <c r="E40" t="n">
-        <v>11.31</v>
+        <v>22.78</v>
       </c>
       <c r="F40" t="n">
-        <v>2.38</v>
+        <v>9.44</v>
       </c>
       <c r="G40" t="n">
-        <v>3.57</v>
+        <v>12.22</v>
       </c>
       <c r="H40" t="n">
-        <v>2.38</v>
+        <v>0</v>
       </c>
       <c r="I40" t="n">
         <v>0</v>
@@ -1826,26 +1826,26 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t xml:space="preserve">Range Rover Sport 2022 </t>
+          <t xml:space="preserve">Isuzu D MAX Crew Cab 2022 </t>
         </is>
       </c>
       <c r="B41" t="n">
         <v>0</v>
       </c>
       <c r="C41" t="n">
-        <v>31.67</v>
+        <v>14.2</v>
       </c>
       <c r="D41" t="n">
-        <v>23.89</v>
+        <v>51.85</v>
       </c>
       <c r="E41" t="n">
-        <v>22.78</v>
+        <v>22.84</v>
       </c>
       <c r="F41" t="n">
-        <v>9.44</v>
+        <v>8.640000000000001</v>
       </c>
       <c r="G41" t="n">
-        <v>12.22</v>
+        <v>2.47</v>
       </c>
       <c r="H41" t="n">
         <v>0</v>
@@ -1860,26 +1860,26 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t xml:space="preserve">Isuzu D MAX Crew Cab 2022 </t>
+          <t xml:space="preserve">NIO ET7 2022 </t>
         </is>
       </c>
       <c r="B42" t="n">
         <v>0</v>
       </c>
       <c r="C42" t="n">
-        <v>14.2</v>
+        <v>22.53</v>
       </c>
       <c r="D42" t="n">
-        <v>51.85</v>
+        <v>46.7</v>
       </c>
       <c r="E42" t="n">
-        <v>22.84</v>
+        <v>12.64</v>
       </c>
       <c r="F42" t="n">
-        <v>8.640000000000001</v>
+        <v>7.69</v>
       </c>
       <c r="G42" t="n">
-        <v>2.47</v>
+        <v>10.44</v>
       </c>
       <c r="H42" t="n">
         <v>0</v>
@@ -1894,26 +1894,26 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t xml:space="preserve">NIO ET7 2022 </t>
+          <t xml:space="preserve">Range Rover 2022 </t>
         </is>
       </c>
       <c r="B43" t="n">
         <v>0</v>
       </c>
       <c r="C43" t="n">
-        <v>22.53</v>
+        <v>26.67</v>
       </c>
       <c r="D43" t="n">
-        <v>46.7</v>
+        <v>38.33</v>
       </c>
       <c r="E43" t="n">
-        <v>12.64</v>
+        <v>17.78</v>
       </c>
       <c r="F43" t="n">
-        <v>7.69</v>
+        <v>6.11</v>
       </c>
       <c r="G43" t="n">
-        <v>10.44</v>
+        <v>11.11</v>
       </c>
       <c r="H43" t="n">
         <v>0</v>
@@ -1928,29 +1928,29 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t xml:space="preserve">Range Rover 2022 </t>
+          <t xml:space="preserve">Renault Austral 2022 </t>
         </is>
       </c>
       <c r="B44" t="n">
         <v>0</v>
       </c>
       <c r="C44" t="n">
-        <v>26.67</v>
+        <v>19.05</v>
       </c>
       <c r="D44" t="n">
-        <v>38.33</v>
+        <v>25.6</v>
       </c>
       <c r="E44" t="n">
-        <v>17.78</v>
+        <v>30.95</v>
       </c>
       <c r="F44" t="n">
-        <v>6.11</v>
+        <v>10.12</v>
       </c>
       <c r="G44" t="n">
-        <v>11.11</v>
+        <v>10.71</v>
       </c>
       <c r="H44" t="n">
-        <v>0</v>
+        <v>3.57</v>
       </c>
       <c r="I44" t="n">
         <v>0</v>
@@ -1962,29 +1962,29 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t xml:space="preserve">Renault Austral 2022 </t>
+          <t xml:space="preserve">DS 9 2022 </t>
         </is>
       </c>
       <c r="B45" t="n">
         <v>0</v>
       </c>
       <c r="C45" t="n">
-        <v>19.05</v>
+        <v>51.76</v>
       </c>
       <c r="D45" t="n">
-        <v>25.6</v>
+        <v>18.24</v>
       </c>
       <c r="E45" t="n">
-        <v>30.95</v>
+        <v>7.06</v>
       </c>
       <c r="F45" t="n">
-        <v>10.12</v>
+        <v>2.94</v>
       </c>
       <c r="G45" t="n">
-        <v>10.71</v>
+        <v>17.65</v>
       </c>
       <c r="H45" t="n">
-        <v>3.57</v>
+        <v>2.35</v>
       </c>
       <c r="I45" t="n">
         <v>0</v>
@@ -1996,29 +1996,29 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t xml:space="preserve">DS 9 2022 </t>
+          <t xml:space="preserve">Tesla Model S 2022 </t>
         </is>
       </c>
       <c r="B46" t="n">
         <v>0</v>
       </c>
       <c r="C46" t="n">
-        <v>51.76</v>
+        <v>35.57</v>
       </c>
       <c r="D46" t="n">
-        <v>18.24</v>
+        <v>41.24</v>
       </c>
       <c r="E46" t="n">
-        <v>7.06</v>
+        <v>5.67</v>
       </c>
       <c r="F46" t="n">
-        <v>2.94</v>
+        <v>4.64</v>
       </c>
       <c r="G46" t="n">
-        <v>17.65</v>
+        <v>10.82</v>
       </c>
       <c r="H46" t="n">
-        <v>2.35</v>
+        <v>2.06</v>
       </c>
       <c r="I46" t="n">
         <v>0</v>
@@ -2030,29 +2030,29 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t xml:space="preserve">Tesla Model S 2022 </t>
+          <t xml:space="preserve">Honda Civic 2022 </t>
         </is>
       </c>
       <c r="B47" t="n">
         <v>0</v>
       </c>
       <c r="C47" t="n">
-        <v>35.57</v>
+        <v>41.76</v>
       </c>
       <c r="D47" t="n">
-        <v>41.24</v>
+        <v>35.88</v>
       </c>
       <c r="E47" t="n">
-        <v>5.67</v>
+        <v>7.06</v>
       </c>
       <c r="F47" t="n">
-        <v>4.64</v>
+        <v>4.71</v>
       </c>
       <c r="G47" t="n">
-        <v>10.82</v>
+        <v>7.06</v>
       </c>
       <c r="H47" t="n">
-        <v>2.06</v>
+        <v>3.53</v>
       </c>
       <c r="I47" t="n">
         <v>0</v>
@@ -2064,29 +2064,29 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t xml:space="preserve">Honda Civic 2022 </t>
+          <t xml:space="preserve">Nissan X Trail 2021 </t>
         </is>
       </c>
       <c r="B48" t="n">
         <v>0</v>
       </c>
       <c r="C48" t="n">
-        <v>41.76</v>
+        <v>32.94</v>
       </c>
       <c r="D48" t="n">
-        <v>35.88</v>
+        <v>34.12</v>
       </c>
       <c r="E48" t="n">
+        <v>12.35</v>
+      </c>
+      <c r="F48" t="n">
         <v>7.06</v>
       </c>
-      <c r="F48" t="n">
-        <v>4.71</v>
-      </c>
       <c r="G48" t="n">
-        <v>7.06</v>
+        <v>11.18</v>
       </c>
       <c r="H48" t="n">
-        <v>3.53</v>
+        <v>2.35</v>
       </c>
       <c r="I48" t="n">
         <v>0</v>
@@ -2098,29 +2098,29 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t xml:space="preserve">Nissan X Trail 2021 </t>
+          <t xml:space="preserve">WEY Coffee 02 2022 </t>
         </is>
       </c>
       <c r="B49" t="n">
         <v>0</v>
       </c>
       <c r="C49" t="n">
-        <v>32.94</v>
+        <v>27.22</v>
       </c>
       <c r="D49" t="n">
-        <v>34.12</v>
+        <v>32.22</v>
       </c>
       <c r="E49" t="n">
-        <v>12.35</v>
+        <v>23.33</v>
       </c>
       <c r="F49" t="n">
-        <v>7.06</v>
+        <v>7.22</v>
       </c>
       <c r="G49" t="n">
-        <v>11.18</v>
+        <v>10</v>
       </c>
       <c r="H49" t="n">
-        <v>2.35</v>
+        <v>0</v>
       </c>
       <c r="I49" t="n">
         <v>0</v>
@@ -2132,29 +2132,29 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t xml:space="preserve">WEY Coffee 02 2022 </t>
+          <t xml:space="preserve">Toyota bZ4X 2022 </t>
         </is>
       </c>
       <c r="B50" t="n">
         <v>0</v>
       </c>
       <c r="C50" t="n">
-        <v>27.22</v>
+        <v>35.06</v>
       </c>
       <c r="D50" t="n">
-        <v>32.22</v>
+        <v>28.16</v>
       </c>
       <c r="E50" t="n">
-        <v>23.33</v>
+        <v>22.99</v>
       </c>
       <c r="F50" t="n">
-        <v>7.22</v>
+        <v>4.6</v>
       </c>
       <c r="G50" t="n">
-        <v>10</v>
+        <v>5.75</v>
       </c>
       <c r="H50" t="n">
-        <v>0</v>
+        <v>3.45</v>
       </c>
       <c r="I50" t="n">
         <v>0</v>
@@ -2166,29 +2166,29 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t xml:space="preserve">Toyota bZ4X 2022 </t>
+          <t xml:space="preserve">SEAT Ibiza 2022 </t>
         </is>
       </c>
       <c r="B51" t="n">
-        <v>0</v>
+        <v>11.11</v>
       </c>
       <c r="C51" t="n">
-        <v>35.06</v>
+        <v>16.05</v>
       </c>
       <c r="D51" t="n">
-        <v>28.16</v>
+        <v>26.54</v>
       </c>
       <c r="E51" t="n">
-        <v>22.99</v>
+        <v>24.07</v>
       </c>
       <c r="F51" t="n">
-        <v>4.6</v>
+        <v>5.56</v>
       </c>
       <c r="G51" t="n">
-        <v>5.75</v>
+        <v>10.49</v>
       </c>
       <c r="H51" t="n">
-        <v>3.45</v>
+        <v>6.17</v>
       </c>
       <c r="I51" t="n">
         <v>0</v>
@@ -2200,29 +2200,29 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t xml:space="preserve">SEAT Ibiza 2022 </t>
+          <t xml:space="preserve">BMW X1 2022 </t>
         </is>
       </c>
       <c r="B52" t="n">
-        <v>11.11</v>
+        <v>0</v>
       </c>
       <c r="C52" t="n">
-        <v>16.05</v>
+        <v>47.53</v>
       </c>
       <c r="D52" t="n">
-        <v>26.54</v>
+        <v>32.72</v>
       </c>
       <c r="E52" t="n">
-        <v>24.07</v>
+        <v>4.94</v>
       </c>
       <c r="F52" t="n">
-        <v>5.56</v>
+        <v>4.32</v>
       </c>
       <c r="G52" t="n">
-        <v>10.49</v>
+        <v>9.26</v>
       </c>
       <c r="H52" t="n">
-        <v>6.17</v>
+        <v>1.23</v>
       </c>
       <c r="I52" t="n">
         <v>0</v>
@@ -2234,29 +2234,29 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t xml:space="preserve">BMW X1 2022 </t>
+          <t xml:space="preserve">Mobilize Limo 2022 </t>
         </is>
       </c>
       <c r="B53" t="n">
-        <v>0</v>
+        <v>5.29</v>
       </c>
       <c r="C53" t="n">
-        <v>47.53</v>
+        <v>14.12</v>
       </c>
       <c r="D53" t="n">
-        <v>32.72</v>
+        <v>33.53</v>
       </c>
       <c r="E53" t="n">
-        <v>4.94</v>
+        <v>15.29</v>
       </c>
       <c r="F53" t="n">
-        <v>4.32</v>
+        <v>8.82</v>
       </c>
       <c r="G53" t="n">
-        <v>9.26</v>
+        <v>18.24</v>
       </c>
       <c r="H53" t="n">
-        <v>1.23</v>
+        <v>4.71</v>
       </c>
       <c r="I53" t="n">
         <v>0</v>
@@ -2268,29 +2268,29 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t xml:space="preserve">Mobilize Limo 2022 </t>
+          <t xml:space="preserve">Mercedes EQ EQE 2022 </t>
         </is>
       </c>
       <c r="B54" t="n">
-        <v>5.29</v>
+        <v>0</v>
       </c>
       <c r="C54" t="n">
-        <v>14.12</v>
+        <v>44.02</v>
       </c>
       <c r="D54" t="n">
-        <v>33.53</v>
+        <v>30.43</v>
       </c>
       <c r="E54" t="n">
-        <v>15.29</v>
+        <v>9.24</v>
       </c>
       <c r="F54" t="n">
-        <v>8.82</v>
+        <v>2.72</v>
       </c>
       <c r="G54" t="n">
-        <v>18.24</v>
+        <v>10.33</v>
       </c>
       <c r="H54" t="n">
-        <v>4.71</v>
+        <v>3.26</v>
       </c>
       <c r="I54" t="n">
         <v>0</v>
@@ -2302,29 +2302,29 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t xml:space="preserve">Mercedes EQ EQE 2022 </t>
+          <t xml:space="preserve">BYD ATTO 3 2022 </t>
         </is>
       </c>
       <c r="B55" t="n">
         <v>0</v>
       </c>
       <c r="C55" t="n">
-        <v>44.02</v>
+        <v>21.51</v>
       </c>
       <c r="D55" t="n">
-        <v>30.43</v>
+        <v>36.63</v>
       </c>
       <c r="E55" t="n">
-        <v>9.24</v>
+        <v>18.02</v>
       </c>
       <c r="F55" t="n">
-        <v>2.72</v>
+        <v>8.720000000000001</v>
       </c>
       <c r="G55" t="n">
-        <v>10.33</v>
+        <v>11.63</v>
       </c>
       <c r="H55" t="n">
-        <v>3.26</v>
+        <v>3.49</v>
       </c>
       <c r="I55" t="n">
         <v>0</v>
@@ -2336,29 +2336,29 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t xml:space="preserve">BYD ATTO 3 2022 </t>
+          <t xml:space="preserve">Citroen C5 X 2022 </t>
         </is>
       </c>
       <c r="B56" t="n">
         <v>0</v>
       </c>
       <c r="C56" t="n">
-        <v>21.51</v>
+        <v>60</v>
       </c>
       <c r="D56" t="n">
-        <v>36.63</v>
+        <v>19.41</v>
       </c>
       <c r="E56" t="n">
-        <v>18.02</v>
+        <v>1.18</v>
       </c>
       <c r="F56" t="n">
-        <v>8.720000000000001</v>
+        <v>2.35</v>
       </c>
       <c r="G56" t="n">
-        <v>11.63</v>
+        <v>14.71</v>
       </c>
       <c r="H56" t="n">
-        <v>3.49</v>
+        <v>2.35</v>
       </c>
       <c r="I56" t="n">
         <v>0</v>
@@ -2370,29 +2370,29 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t xml:space="preserve">Citroen C5 X 2022 </t>
+          <t xml:space="preserve">SEAT Arona 2022 </t>
         </is>
       </c>
       <c r="B57" t="n">
-        <v>0</v>
+        <v>5.56</v>
       </c>
       <c r="C57" t="n">
-        <v>60</v>
+        <v>23.46</v>
       </c>
       <c r="D57" t="n">
-        <v>19.41</v>
+        <v>28.4</v>
       </c>
       <c r="E57" t="n">
-        <v>1.18</v>
+        <v>20.37</v>
       </c>
       <c r="F57" t="n">
-        <v>2.35</v>
+        <v>8.02</v>
       </c>
       <c r="G57" t="n">
-        <v>14.71</v>
+        <v>9.26</v>
       </c>
       <c r="H57" t="n">
-        <v>2.35</v>
+        <v>4.94</v>
       </c>
       <c r="I57" t="n">
         <v>0</v>
@@ -2404,29 +2404,29 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t xml:space="preserve">SEAT Arona 2022 </t>
+          <t xml:space="preserve">MAZDA CX 60 2022 </t>
         </is>
       </c>
       <c r="B58" t="n">
-        <v>5.56</v>
+        <v>0</v>
       </c>
       <c r="C58" t="n">
-        <v>23.46</v>
+        <v>61.59</v>
       </c>
       <c r="D58" t="n">
-        <v>28.4</v>
+        <v>24.39</v>
       </c>
       <c r="E58" t="n">
-        <v>20.37</v>
+        <v>7.32</v>
       </c>
       <c r="F58" t="n">
-        <v>8.02</v>
+        <v>6.71</v>
       </c>
       <c r="G58" t="n">
-        <v>9.26</v>
+        <v>0</v>
       </c>
       <c r="H58" t="n">
-        <v>4.94</v>
+        <v>0</v>
       </c>
       <c r="I58" t="n">
         <v>0</v>
@@ -2438,29 +2438,29 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t xml:space="preserve">MAZDA CX 60 2022 </t>
+          <t xml:space="preserve">BMW 2 Series Active Tourer 2022 </t>
         </is>
       </c>
       <c r="B59" t="n">
-        <v>0</v>
+        <v>5.36</v>
       </c>
       <c r="C59" t="n">
-        <v>61.59</v>
+        <v>39.29</v>
       </c>
       <c r="D59" t="n">
-        <v>24.39</v>
+        <v>21.43</v>
       </c>
       <c r="E59" t="n">
-        <v>7.32</v>
+        <v>7.74</v>
       </c>
       <c r="F59" t="n">
-        <v>6.71</v>
+        <v>3.57</v>
       </c>
       <c r="G59" t="n">
-        <v>0</v>
+        <v>17.86</v>
       </c>
       <c r="H59" t="n">
-        <v>0</v>
+        <v>4.76</v>
       </c>
       <c r="I59" t="n">
         <v>0</v>
@@ -2472,29 +2472,29 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t xml:space="preserve">BMW 2 Series Active Tourer 2022 </t>
+          <t xml:space="preserve">VW Golf 2022 </t>
         </is>
       </c>
       <c r="B60" t="n">
-        <v>5.36</v>
+        <v>5</v>
       </c>
       <c r="C60" t="n">
-        <v>39.29</v>
+        <v>26.88</v>
       </c>
       <c r="D60" t="n">
-        <v>21.43</v>
+        <v>41.88</v>
       </c>
       <c r="E60" t="n">
-        <v>7.74</v>
+        <v>12.5</v>
       </c>
       <c r="F60" t="n">
-        <v>3.57</v>
+        <v>5</v>
       </c>
       <c r="G60" t="n">
-        <v>17.86</v>
+        <v>3.75</v>
       </c>
       <c r="H60" t="n">
-        <v>4.76</v>
+        <v>5</v>
       </c>
       <c r="I60" t="n">
         <v>0</v>
@@ -2506,29 +2506,29 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t xml:space="preserve">VW Golf 2022 </t>
+          <t xml:space="preserve">Kia Sportage 2022 </t>
         </is>
       </c>
       <c r="B61" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C61" t="n">
-        <v>26.88</v>
+        <v>40</v>
       </c>
       <c r="D61" t="n">
-        <v>41.88</v>
+        <v>20.59</v>
       </c>
       <c r="E61" t="n">
-        <v>12.5</v>
+        <v>20</v>
       </c>
       <c r="F61" t="n">
-        <v>5</v>
+        <v>7.65</v>
       </c>
       <c r="G61" t="n">
-        <v>3.75</v>
+        <v>9.41</v>
       </c>
       <c r="H61" t="n">
-        <v>5</v>
+        <v>2.35</v>
       </c>
       <c r="I61" t="n">
         <v>0</v>
@@ -2540,29 +2540,29 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t xml:space="preserve">Kia Sportage 2022 </t>
+          <t xml:space="preserve">BMW i4 2022 </t>
         </is>
       </c>
       <c r="B62" t="n">
         <v>0</v>
       </c>
       <c r="C62" t="n">
-        <v>40</v>
+        <v>64.84</v>
       </c>
       <c r="D62" t="n">
-        <v>20.59</v>
+        <v>23.63</v>
       </c>
       <c r="E62" t="n">
-        <v>20</v>
+        <v>7.69</v>
       </c>
       <c r="F62" t="n">
-        <v>7.65</v>
+        <v>1.65</v>
       </c>
       <c r="G62" t="n">
-        <v>9.41</v>
+        <v>2.2</v>
       </c>
       <c r="H62" t="n">
-        <v>2.35</v>
+        <v>0</v>
       </c>
       <c r="I62" t="n">
         <v>0</v>
@@ -2574,29 +2574,29 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t xml:space="preserve">BMW i4 2022 </t>
+          <t xml:space="preserve">Mercedes Benz T Class 2022 </t>
         </is>
       </c>
       <c r="B63" t="n">
-        <v>0</v>
+        <v>10.34</v>
       </c>
       <c r="C63" t="n">
-        <v>64.84</v>
+        <v>9.77</v>
       </c>
       <c r="D63" t="n">
-        <v>23.63</v>
+        <v>34.48</v>
       </c>
       <c r="E63" t="n">
-        <v>7.69</v>
+        <v>24.71</v>
       </c>
       <c r="F63" t="n">
-        <v>1.65</v>
+        <v>8.050000000000001</v>
       </c>
       <c r="G63" t="n">
-        <v>2.2</v>
+        <v>6.9</v>
       </c>
       <c r="H63" t="n">
-        <v>0</v>
+        <v>5.75</v>
       </c>
       <c r="I63" t="n">
         <v>0</v>
@@ -2608,29 +2608,29 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t xml:space="preserve">Mercedes Benz T Class 2022 </t>
+          <t xml:space="preserve">Toyota Aygo X 2022 </t>
         </is>
       </c>
       <c r="B64" t="n">
-        <v>10.34</v>
+        <v>11.84</v>
       </c>
       <c r="C64" t="n">
-        <v>9.77</v>
+        <v>29.61</v>
       </c>
       <c r="D64" t="n">
-        <v>34.48</v>
+        <v>34.21</v>
       </c>
       <c r="E64" t="n">
-        <v>24.71</v>
+        <v>10.53</v>
       </c>
       <c r="F64" t="n">
-        <v>8.050000000000001</v>
+        <v>0.66</v>
       </c>
       <c r="G64" t="n">
-        <v>6.9</v>
+        <v>7.89</v>
       </c>
       <c r="H64" t="n">
-        <v>5.75</v>
+        <v>5.26</v>
       </c>
       <c r="I64" t="n">
         <v>0</v>
@@ -2642,29 +2642,29 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t xml:space="preserve">Toyota Aygo X 2022 </t>
+          <t xml:space="preserve">Alfa Romeo Tonale 2022 </t>
         </is>
       </c>
       <c r="B65" t="n">
-        <v>11.84</v>
+        <v>0</v>
       </c>
       <c r="C65" t="n">
-        <v>29.61</v>
+        <v>22.02</v>
       </c>
       <c r="D65" t="n">
-        <v>34.21</v>
+        <v>29.76</v>
       </c>
       <c r="E65" t="n">
-        <v>10.53</v>
+        <v>16.67</v>
       </c>
       <c r="F65" t="n">
-        <v>0.66</v>
+        <v>11.9</v>
       </c>
       <c r="G65" t="n">
-        <v>7.89</v>
+        <v>17.26</v>
       </c>
       <c r="H65" t="n">
-        <v>5.26</v>
+        <v>2.38</v>
       </c>
       <c r="I65" t="n">
         <v>0</v>
@@ -2676,68 +2676,34 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t xml:space="preserve">Alfa Romeo Tonale 2022 </t>
+          <t xml:space="preserve">Cupra Born 2022 </t>
         </is>
       </c>
       <c r="B66" t="n">
-        <v>0</v>
+        <v>12.35</v>
       </c>
       <c r="C66" t="n">
-        <v>22.02</v>
+        <v>19.75</v>
       </c>
       <c r="D66" t="n">
-        <v>29.76</v>
+        <v>27.16</v>
       </c>
       <c r="E66" t="n">
-        <v>16.67</v>
+        <v>18.52</v>
       </c>
       <c r="F66" t="n">
-        <v>11.9</v>
+        <v>6.17</v>
       </c>
       <c r="G66" t="n">
-        <v>17.26</v>
+        <v>9.880000000000001</v>
       </c>
       <c r="H66" t="n">
-        <v>2.38</v>
+        <v>6.17</v>
       </c>
       <c r="I66" t="n">
         <v>0</v>
       </c>
       <c r="J66" t="n">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="67">
-      <c r="A67" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Cupra Born 2022 </t>
-        </is>
-      </c>
-      <c r="B67" t="n">
-        <v>12.35</v>
-      </c>
-      <c r="C67" t="n">
-        <v>19.75</v>
-      </c>
-      <c r="D67" t="n">
-        <v>27.16</v>
-      </c>
-      <c r="E67" t="n">
-        <v>18.52</v>
-      </c>
-      <c r="F67" t="n">
-        <v>6.17</v>
-      </c>
-      <c r="G67" t="n">
-        <v>9.880000000000001</v>
-      </c>
-      <c r="H67" t="n">
-        <v>6.17</v>
-      </c>
-      <c r="I67" t="n">
-        <v>0</v>
-      </c>
-      <c r="J67" t="n">
         <v>100</v>
       </c>
     </row>

</xml_diff>